<commit_message>
Removed logo; Added Creative Commons
</commit_message>
<xml_diff>
--- a/MetadataCompilation.xlsx
+++ b/MetadataCompilation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="60" windowWidth="26265" windowHeight="7710" tabRatio="826" activeTab="3"/>
+    <workbookView xWindow="450" yWindow="60" windowWidth="26265" windowHeight="7710" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2012,7 +2012,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="432">
   <si>
     <t>Title</t>
   </si>
@@ -3356,6 +3356,9 @@
   <si>
     <t>Data History</t>
   </si>
+  <si>
+    <t>Copyright © Arizona Geological Survey, 2012</t>
+  </si>
 </sst>
 </file>
 
@@ -3367,7 +3370,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\Thh:mm"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="71">
+  <fonts count="72">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3847,6 +3850,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -4917,7 +4926,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="347">
+  <cellStyleXfs count="346">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4960,7 +4969,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="29" borderId="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5277,7 +5285,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="209">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5612,88 +5620,87 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="55" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="38" xfId="45" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="38" xfId="44" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="56"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="55"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="55" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="44" borderId="39" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="44" borderId="39" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="55" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="40" xfId="56" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="40" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="41" xfId="56" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="35" fillId="0" borderId="41" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="36" fillId="0" borderId="9" xfId="56" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="36" fillId="0" borderId="9" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="40" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="40" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="43" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="43" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="55" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="44" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="44" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="44" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="44" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="56" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="55" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="49" borderId="38" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="35" fillId="49" borderId="38" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5792,30 +5799,30 @@
     <xf numFmtId="165" fontId="25" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="55" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="45" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="45" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="46" borderId="45" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="46" borderId="45" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="46" borderId="46" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="46" borderId="46" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="46" borderId="47" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="46" borderId="47" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="47" borderId="48" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="47" borderId="48" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="47" borderId="49" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="47" borderId="49" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="47" borderId="50" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="47" borderId="50" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5879,355 +5886,358 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="44" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="50" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="347">
+  <cellStyles count="346">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="111"/>
-    <cellStyle name="20% - Accent1 3" xfId="129"/>
-    <cellStyle name="20% - Accent1 3 2" xfId="152"/>
-    <cellStyle name="20% - Accent1 4" xfId="153"/>
-    <cellStyle name="20% - Accent1 5" xfId="151"/>
+    <cellStyle name="20% - Accent1 2" xfId="110"/>
+    <cellStyle name="20% - Accent1 3" xfId="128"/>
+    <cellStyle name="20% - Accent1 3 2" xfId="151"/>
+    <cellStyle name="20% - Accent1 4" xfId="152"/>
+    <cellStyle name="20% - Accent1 5" xfId="150"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="112"/>
-    <cellStyle name="20% - Accent2 3" xfId="130"/>
-    <cellStyle name="20% - Accent2 3 2" xfId="155"/>
-    <cellStyle name="20% - Accent2 4" xfId="156"/>
-    <cellStyle name="20% - Accent2 5" xfId="154"/>
+    <cellStyle name="20% - Accent2 2" xfId="111"/>
+    <cellStyle name="20% - Accent2 3" xfId="129"/>
+    <cellStyle name="20% - Accent2 3 2" xfId="154"/>
+    <cellStyle name="20% - Accent2 4" xfId="155"/>
+    <cellStyle name="20% - Accent2 5" xfId="153"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="113"/>
-    <cellStyle name="20% - Accent3 3" xfId="131"/>
-    <cellStyle name="20% - Accent3 3 2" xfId="158"/>
-    <cellStyle name="20% - Accent3 4" xfId="159"/>
-    <cellStyle name="20% - Accent3 5" xfId="157"/>
+    <cellStyle name="20% - Accent3 2" xfId="112"/>
+    <cellStyle name="20% - Accent3 3" xfId="130"/>
+    <cellStyle name="20% - Accent3 3 2" xfId="157"/>
+    <cellStyle name="20% - Accent3 4" xfId="158"/>
+    <cellStyle name="20% - Accent3 5" xfId="156"/>
     <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="114"/>
-    <cellStyle name="20% - Accent4 3" xfId="132"/>
-    <cellStyle name="20% - Accent4 3 2" xfId="161"/>
-    <cellStyle name="20% - Accent4 4" xfId="162"/>
-    <cellStyle name="20% - Accent4 5" xfId="160"/>
+    <cellStyle name="20% - Accent4 2" xfId="113"/>
+    <cellStyle name="20% - Accent4 3" xfId="131"/>
+    <cellStyle name="20% - Accent4 3 2" xfId="160"/>
+    <cellStyle name="20% - Accent4 4" xfId="161"/>
+    <cellStyle name="20% - Accent4 5" xfId="159"/>
     <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="115"/>
-    <cellStyle name="20% - Accent5 3" xfId="133"/>
-    <cellStyle name="20% - Accent5 4" xfId="163"/>
+    <cellStyle name="20% - Accent5 2" xfId="114"/>
+    <cellStyle name="20% - Accent5 3" xfId="132"/>
+    <cellStyle name="20% - Accent5 4" xfId="162"/>
     <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="116"/>
-    <cellStyle name="20% - Accent6 3" xfId="134"/>
-    <cellStyle name="20% - Accent6 3 2" xfId="165"/>
-    <cellStyle name="20% - Accent6 4" xfId="166"/>
-    <cellStyle name="20% - Accent6 5" xfId="164"/>
+    <cellStyle name="20% - Accent6 2" xfId="115"/>
+    <cellStyle name="20% - Accent6 3" xfId="133"/>
+    <cellStyle name="20% - Accent6 3 2" xfId="164"/>
+    <cellStyle name="20% - Accent6 4" xfId="165"/>
+    <cellStyle name="20% - Accent6 5" xfId="163"/>
     <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="117"/>
-    <cellStyle name="40% - Accent1 3" xfId="135"/>
-    <cellStyle name="40% - Accent1 3 2" xfId="168"/>
-    <cellStyle name="40% - Accent1 4" xfId="169"/>
-    <cellStyle name="40% - Accent1 5" xfId="167"/>
+    <cellStyle name="40% - Accent1 2" xfId="116"/>
+    <cellStyle name="40% - Accent1 3" xfId="134"/>
+    <cellStyle name="40% - Accent1 3 2" xfId="167"/>
+    <cellStyle name="40% - Accent1 4" xfId="168"/>
+    <cellStyle name="40% - Accent1 5" xfId="166"/>
     <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="118"/>
-    <cellStyle name="40% - Accent2 3" xfId="136"/>
-    <cellStyle name="40% - Accent2 4" xfId="170"/>
+    <cellStyle name="40% - Accent2 2" xfId="117"/>
+    <cellStyle name="40% - Accent2 3" xfId="135"/>
+    <cellStyle name="40% - Accent2 4" xfId="169"/>
     <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="119"/>
-    <cellStyle name="40% - Accent3 3" xfId="137"/>
-    <cellStyle name="40% - Accent3 3 2" xfId="172"/>
-    <cellStyle name="40% - Accent3 4" xfId="173"/>
-    <cellStyle name="40% - Accent3 5" xfId="171"/>
+    <cellStyle name="40% - Accent3 2" xfId="118"/>
+    <cellStyle name="40% - Accent3 3" xfId="136"/>
+    <cellStyle name="40% - Accent3 3 2" xfId="171"/>
+    <cellStyle name="40% - Accent3 4" xfId="172"/>
+    <cellStyle name="40% - Accent3 5" xfId="170"/>
     <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="120"/>
-    <cellStyle name="40% - Accent4 3" xfId="138"/>
-    <cellStyle name="40% - Accent4 3 2" xfId="175"/>
-    <cellStyle name="40% - Accent4 4" xfId="176"/>
-    <cellStyle name="40% - Accent4 5" xfId="174"/>
+    <cellStyle name="40% - Accent4 2" xfId="119"/>
+    <cellStyle name="40% - Accent4 3" xfId="137"/>
+    <cellStyle name="40% - Accent4 3 2" xfId="174"/>
+    <cellStyle name="40% - Accent4 4" xfId="175"/>
+    <cellStyle name="40% - Accent4 5" xfId="173"/>
     <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="121"/>
-    <cellStyle name="40% - Accent5 3" xfId="139"/>
-    <cellStyle name="40% - Accent5 3 2" xfId="178"/>
-    <cellStyle name="40% - Accent5 4" xfId="179"/>
-    <cellStyle name="40% - Accent5 5" xfId="177"/>
+    <cellStyle name="40% - Accent5 2" xfId="120"/>
+    <cellStyle name="40% - Accent5 3" xfId="138"/>
+    <cellStyle name="40% - Accent5 3 2" xfId="177"/>
+    <cellStyle name="40% - Accent5 4" xfId="178"/>
+    <cellStyle name="40% - Accent5 5" xfId="176"/>
     <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="122"/>
-    <cellStyle name="40% - Accent6 3" xfId="140"/>
-    <cellStyle name="40% - Accent6 3 2" xfId="181"/>
-    <cellStyle name="40% - Accent6 4" xfId="182"/>
-    <cellStyle name="40% - Accent6 5" xfId="180"/>
+    <cellStyle name="40% - Accent6 2" xfId="121"/>
+    <cellStyle name="40% - Accent6 3" xfId="139"/>
+    <cellStyle name="40% - Accent6 3 2" xfId="180"/>
+    <cellStyle name="40% - Accent6 4" xfId="181"/>
+    <cellStyle name="40% - Accent6 5" xfId="179"/>
     <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1 2" xfId="184"/>
-    <cellStyle name="60% - Accent1 3" xfId="185"/>
-    <cellStyle name="60% - Accent1 3 2" xfId="186"/>
-    <cellStyle name="60% - Accent1 4" xfId="187"/>
-    <cellStyle name="60% - Accent1 5" xfId="183"/>
+    <cellStyle name="60% - Accent1 2" xfId="183"/>
+    <cellStyle name="60% - Accent1 3" xfId="184"/>
+    <cellStyle name="60% - Accent1 3 2" xfId="185"/>
+    <cellStyle name="60% - Accent1 4" xfId="186"/>
+    <cellStyle name="60% - Accent1 5" xfId="182"/>
     <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2 2" xfId="189"/>
-    <cellStyle name="60% - Accent2 3" xfId="190"/>
-    <cellStyle name="60% - Accent2 3 2" xfId="191"/>
-    <cellStyle name="60% - Accent2 4" xfId="192"/>
-    <cellStyle name="60% - Accent2 5" xfId="188"/>
+    <cellStyle name="60% - Accent2 2" xfId="188"/>
+    <cellStyle name="60% - Accent2 3" xfId="189"/>
+    <cellStyle name="60% - Accent2 3 2" xfId="190"/>
+    <cellStyle name="60% - Accent2 4" xfId="191"/>
+    <cellStyle name="60% - Accent2 5" xfId="187"/>
     <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3 2" xfId="194"/>
-    <cellStyle name="60% - Accent3 3" xfId="195"/>
-    <cellStyle name="60% - Accent3 3 2" xfId="196"/>
-    <cellStyle name="60% - Accent3 4" xfId="197"/>
-    <cellStyle name="60% - Accent3 5" xfId="193"/>
+    <cellStyle name="60% - Accent3 2" xfId="193"/>
+    <cellStyle name="60% - Accent3 3" xfId="194"/>
+    <cellStyle name="60% - Accent3 3 2" xfId="195"/>
+    <cellStyle name="60% - Accent3 4" xfId="196"/>
+    <cellStyle name="60% - Accent3 5" xfId="192"/>
     <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4 2" xfId="199"/>
-    <cellStyle name="60% - Accent4 3" xfId="200"/>
-    <cellStyle name="60% - Accent4 3 2" xfId="201"/>
-    <cellStyle name="60% - Accent4 4" xfId="202"/>
-    <cellStyle name="60% - Accent4 5" xfId="198"/>
+    <cellStyle name="60% - Accent4 2" xfId="198"/>
+    <cellStyle name="60% - Accent4 3" xfId="199"/>
+    <cellStyle name="60% - Accent4 3 2" xfId="200"/>
+    <cellStyle name="60% - Accent4 4" xfId="201"/>
+    <cellStyle name="60% - Accent4 5" xfId="197"/>
     <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5 2" xfId="204"/>
-    <cellStyle name="60% - Accent5 3" xfId="205"/>
-    <cellStyle name="60% - Accent5 3 2" xfId="206"/>
-    <cellStyle name="60% - Accent5 4" xfId="207"/>
-    <cellStyle name="60% - Accent5 5" xfId="203"/>
+    <cellStyle name="60% - Accent5 2" xfId="203"/>
+    <cellStyle name="60% - Accent5 3" xfId="204"/>
+    <cellStyle name="60% - Accent5 3 2" xfId="205"/>
+    <cellStyle name="60% - Accent5 4" xfId="206"/>
+    <cellStyle name="60% - Accent5 5" xfId="202"/>
     <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6 2" xfId="209"/>
-    <cellStyle name="60% - Accent6 3" xfId="210"/>
-    <cellStyle name="60% - Accent6 3 2" xfId="211"/>
-    <cellStyle name="60% - Accent6 4" xfId="212"/>
-    <cellStyle name="60% - Accent6 5" xfId="208"/>
+    <cellStyle name="60% - Accent6 2" xfId="208"/>
+    <cellStyle name="60% - Accent6 3" xfId="209"/>
+    <cellStyle name="60% - Accent6 3 2" xfId="210"/>
+    <cellStyle name="60% - Accent6 4" xfId="211"/>
+    <cellStyle name="60% - Accent6 5" xfId="207"/>
     <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent1 2" xfId="214"/>
-    <cellStyle name="Accent1 3" xfId="215"/>
-    <cellStyle name="Accent1 3 2" xfId="216"/>
-    <cellStyle name="Accent1 4" xfId="217"/>
-    <cellStyle name="Accent1 5" xfId="213"/>
+    <cellStyle name="Accent1 2" xfId="213"/>
+    <cellStyle name="Accent1 3" xfId="214"/>
+    <cellStyle name="Accent1 3 2" xfId="215"/>
+    <cellStyle name="Accent1 4" xfId="216"/>
+    <cellStyle name="Accent1 5" xfId="212"/>
     <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent2 2" xfId="219"/>
-    <cellStyle name="Accent2 3" xfId="220"/>
-    <cellStyle name="Accent2 3 2" xfId="221"/>
-    <cellStyle name="Accent2 4" xfId="222"/>
-    <cellStyle name="Accent2 5" xfId="218"/>
+    <cellStyle name="Accent2 2" xfId="218"/>
+    <cellStyle name="Accent2 3" xfId="219"/>
+    <cellStyle name="Accent2 3 2" xfId="220"/>
+    <cellStyle name="Accent2 4" xfId="221"/>
+    <cellStyle name="Accent2 5" xfId="217"/>
     <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent3 2" xfId="224"/>
-    <cellStyle name="Accent3 3" xfId="225"/>
-    <cellStyle name="Accent3 3 2" xfId="226"/>
-    <cellStyle name="Accent3 4" xfId="227"/>
-    <cellStyle name="Accent3 5" xfId="223"/>
+    <cellStyle name="Accent3 2" xfId="223"/>
+    <cellStyle name="Accent3 3" xfId="224"/>
+    <cellStyle name="Accent3 3 2" xfId="225"/>
+    <cellStyle name="Accent3 4" xfId="226"/>
+    <cellStyle name="Accent3 5" xfId="222"/>
     <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent4 2" xfId="229"/>
-    <cellStyle name="Accent4 3" xfId="230"/>
-    <cellStyle name="Accent4 3 2" xfId="231"/>
-    <cellStyle name="Accent4 4" xfId="232"/>
-    <cellStyle name="Accent4 5" xfId="228"/>
+    <cellStyle name="Accent4 2" xfId="228"/>
+    <cellStyle name="Accent4 3" xfId="229"/>
+    <cellStyle name="Accent4 3 2" xfId="230"/>
+    <cellStyle name="Accent4 4" xfId="231"/>
+    <cellStyle name="Accent4 5" xfId="227"/>
     <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent5 2" xfId="234"/>
-    <cellStyle name="Accent5 3" xfId="235"/>
-    <cellStyle name="Accent5 4" xfId="233"/>
+    <cellStyle name="Accent5 2" xfId="233"/>
+    <cellStyle name="Accent5 3" xfId="234"/>
+    <cellStyle name="Accent5 4" xfId="232"/>
     <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Accent6 2" xfId="237"/>
-    <cellStyle name="Accent6 3" xfId="238"/>
-    <cellStyle name="Accent6 3 2" xfId="239"/>
-    <cellStyle name="Accent6 4" xfId="240"/>
-    <cellStyle name="Accent6 5" xfId="236"/>
+    <cellStyle name="Accent6 2" xfId="236"/>
+    <cellStyle name="Accent6 3" xfId="237"/>
+    <cellStyle name="Accent6 3 2" xfId="238"/>
+    <cellStyle name="Accent6 4" xfId="239"/>
+    <cellStyle name="Accent6 5" xfId="235"/>
     <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Bad 2" xfId="242"/>
-    <cellStyle name="Bad 3" xfId="243"/>
-    <cellStyle name="Bad 3 2" xfId="244"/>
-    <cellStyle name="Bad 4" xfId="245"/>
-    <cellStyle name="Bad 5" xfId="241"/>
+    <cellStyle name="Bad 2" xfId="241"/>
+    <cellStyle name="Bad 3" xfId="242"/>
+    <cellStyle name="Bad 3 2" xfId="243"/>
+    <cellStyle name="Bad 4" xfId="244"/>
+    <cellStyle name="Bad 5" xfId="240"/>
     <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Calculation 2" xfId="247"/>
-    <cellStyle name="Calculation 3" xfId="248"/>
-    <cellStyle name="Calculation 3 2" xfId="249"/>
-    <cellStyle name="Calculation 4" xfId="250"/>
-    <cellStyle name="Calculation 5" xfId="246"/>
+    <cellStyle name="Calculation 2" xfId="246"/>
+    <cellStyle name="Calculation 3" xfId="247"/>
+    <cellStyle name="Calculation 3 2" xfId="248"/>
+    <cellStyle name="Calculation 4" xfId="249"/>
+    <cellStyle name="Calculation 5" xfId="245"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Check Cell 2" xfId="252"/>
-    <cellStyle name="Check Cell 3" xfId="253"/>
-    <cellStyle name="Check Cell 4" xfId="251"/>
-    <cellStyle name="Comma 2" xfId="254"/>
-    <cellStyle name="depth" xfId="43"/>
+    <cellStyle name="Check Cell 2" xfId="251"/>
+    <cellStyle name="Check Cell 3" xfId="252"/>
+    <cellStyle name="Check Cell 4" xfId="250"/>
+    <cellStyle name="Comma 2" xfId="253"/>
+    <cellStyle name="depth" xfId="42"/>
     <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text 2" xfId="256"/>
-    <cellStyle name="Explanatory Text 3" xfId="257"/>
-    <cellStyle name="Explanatory Text 4" xfId="255"/>
+    <cellStyle name="Explanatory Text 2" xfId="255"/>
+    <cellStyle name="Explanatory Text 3" xfId="256"/>
+    <cellStyle name="Explanatory Text 4" xfId="254"/>
     <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Good 2" xfId="259"/>
-    <cellStyle name="Good 3" xfId="260"/>
-    <cellStyle name="Good 3 2" xfId="261"/>
-    <cellStyle name="Good 4" xfId="262"/>
-    <cellStyle name="Good 5" xfId="258"/>
+    <cellStyle name="Good 2" xfId="258"/>
+    <cellStyle name="Good 3" xfId="259"/>
+    <cellStyle name="Good 3 2" xfId="260"/>
+    <cellStyle name="Good 4" xfId="261"/>
+    <cellStyle name="Good 5" xfId="257"/>
     <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 1 2" xfId="264"/>
-    <cellStyle name="Heading 1 3" xfId="265"/>
-    <cellStyle name="Heading 1 3 2" xfId="266"/>
-    <cellStyle name="Heading 1 4" xfId="267"/>
-    <cellStyle name="Heading 1 5" xfId="263"/>
+    <cellStyle name="Heading 1 2" xfId="263"/>
+    <cellStyle name="Heading 1 3" xfId="264"/>
+    <cellStyle name="Heading 1 3 2" xfId="265"/>
+    <cellStyle name="Heading 1 4" xfId="266"/>
+    <cellStyle name="Heading 1 5" xfId="262"/>
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 2 2" xfId="269"/>
-    <cellStyle name="Heading 2 3" xfId="270"/>
-    <cellStyle name="Heading 2 3 2" xfId="271"/>
-    <cellStyle name="Heading 2 4" xfId="272"/>
-    <cellStyle name="Heading 2 5" xfId="268"/>
+    <cellStyle name="Heading 2 2" xfId="268"/>
+    <cellStyle name="Heading 2 3" xfId="269"/>
+    <cellStyle name="Heading 2 3 2" xfId="270"/>
+    <cellStyle name="Heading 2 4" xfId="271"/>
+    <cellStyle name="Heading 2 5" xfId="267"/>
     <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 3 2" xfId="274"/>
-    <cellStyle name="Heading 3 3" xfId="275"/>
-    <cellStyle name="Heading 3 3 2" xfId="276"/>
-    <cellStyle name="Heading 3 4" xfId="277"/>
-    <cellStyle name="Heading 3 5" xfId="273"/>
+    <cellStyle name="Heading 3 2" xfId="273"/>
+    <cellStyle name="Heading 3 3" xfId="274"/>
+    <cellStyle name="Heading 3 3 2" xfId="275"/>
+    <cellStyle name="Heading 3 4" xfId="276"/>
+    <cellStyle name="Heading 3 5" xfId="272"/>
     <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Heading 4 2" xfId="279"/>
-    <cellStyle name="Heading 4 3" xfId="280"/>
-    <cellStyle name="Heading 4 3 2" xfId="281"/>
-    <cellStyle name="Heading 4 4" xfId="282"/>
-    <cellStyle name="Heading 4 5" xfId="278"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="44"/>
-    <cellStyle name="Hyperlink 2 2" xfId="147"/>
-    <cellStyle name="Hyperlink 3" xfId="45"/>
-    <cellStyle name="Hyperlink 4" xfId="46"/>
-    <cellStyle name="Hyperlink 5" xfId="47"/>
-    <cellStyle name="Hyperlink 6" xfId="94"/>
-    <cellStyle name="Hyperlink 6 2" xfId="284"/>
-    <cellStyle name="Hyperlink 7" xfId="285"/>
+    <cellStyle name="Heading 4 2" xfId="278"/>
+    <cellStyle name="Heading 4 3" xfId="279"/>
+    <cellStyle name="Heading 4 3 2" xfId="280"/>
+    <cellStyle name="Heading 4 4" xfId="281"/>
+    <cellStyle name="Heading 4 5" xfId="277"/>
+    <cellStyle name="Hyperlink 2" xfId="43"/>
+    <cellStyle name="Hyperlink 2 2" xfId="146"/>
+    <cellStyle name="Hyperlink 3" xfId="44"/>
+    <cellStyle name="Hyperlink 4" xfId="45"/>
+    <cellStyle name="Hyperlink 5" xfId="46"/>
+    <cellStyle name="Hyperlink 6" xfId="93"/>
+    <cellStyle name="Hyperlink 6 2" xfId="283"/>
+    <cellStyle name="Hyperlink 7" xfId="284"/>
     <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Input 2" xfId="287"/>
-    <cellStyle name="Input 3" xfId="288"/>
-    <cellStyle name="Input 3 2" xfId="289"/>
-    <cellStyle name="Input 4" xfId="290"/>
-    <cellStyle name="Input 5" xfId="286"/>
+    <cellStyle name="Input 2" xfId="286"/>
+    <cellStyle name="Input 3" xfId="287"/>
+    <cellStyle name="Input 3 2" xfId="288"/>
+    <cellStyle name="Input 4" xfId="289"/>
+    <cellStyle name="Input 5" xfId="285"/>
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Linked Cell 2" xfId="292"/>
-    <cellStyle name="Linked Cell 3" xfId="293"/>
-    <cellStyle name="Linked Cell 3 2" xfId="294"/>
-    <cellStyle name="Linked Cell 4" xfId="295"/>
-    <cellStyle name="Linked Cell 5" xfId="291"/>
+    <cellStyle name="Linked Cell 2" xfId="291"/>
+    <cellStyle name="Linked Cell 3" xfId="292"/>
+    <cellStyle name="Linked Cell 3 2" xfId="293"/>
+    <cellStyle name="Linked Cell 4" xfId="294"/>
+    <cellStyle name="Linked Cell 5" xfId="290"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="297"/>
-    <cellStyle name="Neutral 3" xfId="298"/>
-    <cellStyle name="Neutral 3 2" xfId="299"/>
-    <cellStyle name="Neutral 4" xfId="300"/>
-    <cellStyle name="Neutral 5" xfId="296"/>
+    <cellStyle name="Neutral 2" xfId="296"/>
+    <cellStyle name="Neutral 3" xfId="297"/>
+    <cellStyle name="Neutral 3 2" xfId="298"/>
+    <cellStyle name="Neutral 4" xfId="299"/>
+    <cellStyle name="Neutral 5" xfId="295"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="48"/>
-    <cellStyle name="Normal 11" xfId="49"/>
-    <cellStyle name="Normal 11 2" xfId="50"/>
-    <cellStyle name="Normal 11 3" xfId="301"/>
-    <cellStyle name="Normal 11 4" xfId="100"/>
-    <cellStyle name="Normal 12" xfId="302"/>
-    <cellStyle name="Normal 13" xfId="303"/>
-    <cellStyle name="Normal 13 2" xfId="95"/>
-    <cellStyle name="Normal 13 2 2" xfId="123"/>
-    <cellStyle name="Normal 13 2 3" xfId="141"/>
-    <cellStyle name="Normal 13 3" xfId="96"/>
-    <cellStyle name="Normal 13 3 2" xfId="124"/>
-    <cellStyle name="Normal 13 3 3" xfId="142"/>
-    <cellStyle name="Normal 14" xfId="304"/>
-    <cellStyle name="Normal 15" xfId="150"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Normal 2 10 2 2 2 2" xfId="52"/>
-    <cellStyle name="Normal 2 2" xfId="53"/>
-    <cellStyle name="Normal 2 2 2" xfId="148"/>
-    <cellStyle name="Normal 2 2 3" xfId="97"/>
-    <cellStyle name="Normal 2 3" xfId="54"/>
-    <cellStyle name="Normal 2 3 2" xfId="305"/>
-    <cellStyle name="Normal 2 3 3" xfId="125"/>
-    <cellStyle name="Normal 2 4" xfId="143"/>
-    <cellStyle name="Normal 2 4 2" xfId="149"/>
-    <cellStyle name="Normal 2_DataMappingView" xfId="55"/>
-    <cellStyle name="Normal 3" xfId="56"/>
-    <cellStyle name="Normal 3 2" xfId="57"/>
-    <cellStyle name="Normal 3 2 2" xfId="58"/>
-    <cellStyle name="Normal 3 2 3" xfId="59"/>
-    <cellStyle name="Normal 3 2 4" xfId="60"/>
-    <cellStyle name="Normal 3 2 5" xfId="307"/>
-    <cellStyle name="Normal 3 2 6" xfId="102"/>
-    <cellStyle name="Normal 3 2_DataMappingView" xfId="61"/>
-    <cellStyle name="Normal 3 3" xfId="62"/>
-    <cellStyle name="Normal 3 3 2" xfId="308"/>
-    <cellStyle name="Normal 3 3 3" xfId="101"/>
-    <cellStyle name="Normal 3 4" xfId="63"/>
-    <cellStyle name="Normal 3 5" xfId="64"/>
-    <cellStyle name="Normal 3 6" xfId="306"/>
-    <cellStyle name="Normal 3 7" xfId="98"/>
-    <cellStyle name="Normal 3 8" xfId="283"/>
-    <cellStyle name="Normal 3 9" xfId="346"/>
-    <cellStyle name="Normal 4" xfId="65"/>
-    <cellStyle name="Normal 4 2" xfId="66"/>
-    <cellStyle name="Normal 4 2 2" xfId="309"/>
-    <cellStyle name="Normal 4 2 3" xfId="104"/>
-    <cellStyle name="Normal 4 3" xfId="67"/>
-    <cellStyle name="Normal 4 3 2" xfId="310"/>
-    <cellStyle name="Normal 4 3 3" xfId="103"/>
-    <cellStyle name="Normal 4 4" xfId="126"/>
-    <cellStyle name="Normal 4 5" xfId="144"/>
-    <cellStyle name="Normal 5" xfId="68"/>
-    <cellStyle name="Normal 5 2" xfId="106"/>
-    <cellStyle name="Normal 5 3" xfId="105"/>
-    <cellStyle name="Normal 5 4" xfId="127"/>
-    <cellStyle name="Normal 5 5" xfId="145"/>
-    <cellStyle name="Normal 6" xfId="69"/>
-    <cellStyle name="Normal 6 2" xfId="108"/>
-    <cellStyle name="Normal 6 3" xfId="107"/>
-    <cellStyle name="Normal 6 4" xfId="128"/>
-    <cellStyle name="Normal 6 5" xfId="146"/>
-    <cellStyle name="Normal 6 6" xfId="311"/>
-    <cellStyle name="Normal 6 7" xfId="99"/>
-    <cellStyle name="Normal 7" xfId="70"/>
-    <cellStyle name="Normal 7 2" xfId="109"/>
-    <cellStyle name="Normal 8" xfId="71"/>
-    <cellStyle name="Normal 9" xfId="72"/>
-    <cellStyle name="Normal 9 2" xfId="312"/>
-    <cellStyle name="Normal 9 3" xfId="110"/>
+    <cellStyle name="Normal 10" xfId="47"/>
+    <cellStyle name="Normal 11" xfId="48"/>
+    <cellStyle name="Normal 11 2" xfId="49"/>
+    <cellStyle name="Normal 11 3" xfId="300"/>
+    <cellStyle name="Normal 11 4" xfId="99"/>
+    <cellStyle name="Normal 12" xfId="301"/>
+    <cellStyle name="Normal 13" xfId="302"/>
+    <cellStyle name="Normal 13 2" xfId="94"/>
+    <cellStyle name="Normal 13 2 2" xfId="122"/>
+    <cellStyle name="Normal 13 2 3" xfId="140"/>
+    <cellStyle name="Normal 13 3" xfId="95"/>
+    <cellStyle name="Normal 13 3 2" xfId="123"/>
+    <cellStyle name="Normal 13 3 3" xfId="141"/>
+    <cellStyle name="Normal 14" xfId="303"/>
+    <cellStyle name="Normal 15" xfId="149"/>
+    <cellStyle name="Normal 2" xfId="50"/>
+    <cellStyle name="Normal 2 10 2 2 2 2" xfId="51"/>
+    <cellStyle name="Normal 2 2" xfId="52"/>
+    <cellStyle name="Normal 2 2 2" xfId="147"/>
+    <cellStyle name="Normal 2 2 3" xfId="96"/>
+    <cellStyle name="Normal 2 3" xfId="53"/>
+    <cellStyle name="Normal 2 3 2" xfId="304"/>
+    <cellStyle name="Normal 2 3 3" xfId="124"/>
+    <cellStyle name="Normal 2 4" xfId="142"/>
+    <cellStyle name="Normal 2 4 2" xfId="148"/>
+    <cellStyle name="Normal 2_DataMappingView" xfId="54"/>
+    <cellStyle name="Normal 3" xfId="55"/>
+    <cellStyle name="Normal 3 2" xfId="56"/>
+    <cellStyle name="Normal 3 2 2" xfId="57"/>
+    <cellStyle name="Normal 3 2 3" xfId="58"/>
+    <cellStyle name="Normal 3 2 4" xfId="59"/>
+    <cellStyle name="Normal 3 2 5" xfId="306"/>
+    <cellStyle name="Normal 3 2 6" xfId="101"/>
+    <cellStyle name="Normal 3 2_DataMappingView" xfId="60"/>
+    <cellStyle name="Normal 3 3" xfId="61"/>
+    <cellStyle name="Normal 3 3 2" xfId="307"/>
+    <cellStyle name="Normal 3 3 3" xfId="100"/>
+    <cellStyle name="Normal 3 4" xfId="62"/>
+    <cellStyle name="Normal 3 5" xfId="63"/>
+    <cellStyle name="Normal 3 6" xfId="305"/>
+    <cellStyle name="Normal 3 7" xfId="97"/>
+    <cellStyle name="Normal 3 8" xfId="282"/>
+    <cellStyle name="Normal 3 9" xfId="345"/>
+    <cellStyle name="Normal 4" xfId="64"/>
+    <cellStyle name="Normal 4 2" xfId="65"/>
+    <cellStyle name="Normal 4 2 2" xfId="308"/>
+    <cellStyle name="Normal 4 2 3" xfId="103"/>
+    <cellStyle name="Normal 4 3" xfId="66"/>
+    <cellStyle name="Normal 4 3 2" xfId="309"/>
+    <cellStyle name="Normal 4 3 3" xfId="102"/>
+    <cellStyle name="Normal 4 4" xfId="125"/>
+    <cellStyle name="Normal 4 5" xfId="143"/>
+    <cellStyle name="Normal 5" xfId="67"/>
+    <cellStyle name="Normal 5 2" xfId="105"/>
+    <cellStyle name="Normal 5 3" xfId="104"/>
+    <cellStyle name="Normal 5 4" xfId="126"/>
+    <cellStyle name="Normal 5 5" xfId="144"/>
+    <cellStyle name="Normal 6" xfId="68"/>
+    <cellStyle name="Normal 6 2" xfId="107"/>
+    <cellStyle name="Normal 6 3" xfId="106"/>
+    <cellStyle name="Normal 6 4" xfId="127"/>
+    <cellStyle name="Normal 6 5" xfId="145"/>
+    <cellStyle name="Normal 6 6" xfId="310"/>
+    <cellStyle name="Normal 6 7" xfId="98"/>
+    <cellStyle name="Normal 7" xfId="69"/>
+    <cellStyle name="Normal 7 2" xfId="108"/>
+    <cellStyle name="Normal 8" xfId="70"/>
+    <cellStyle name="Normal 9" xfId="71"/>
+    <cellStyle name="Normal 9 2" xfId="311"/>
+    <cellStyle name="Normal 9 3" xfId="109"/>
     <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 10" xfId="313"/>
-    <cellStyle name="Note 2" xfId="73"/>
-    <cellStyle name="Note 2 2" xfId="74"/>
-    <cellStyle name="Note 2 3" xfId="314"/>
-    <cellStyle name="Note 3" xfId="75"/>
-    <cellStyle name="Note 4" xfId="76"/>
-    <cellStyle name="Note 5" xfId="77"/>
-    <cellStyle name="Note 6" xfId="315"/>
-    <cellStyle name="Note 6 2" xfId="316"/>
-    <cellStyle name="Note 7" xfId="317"/>
-    <cellStyle name="Note 8" xfId="318"/>
-    <cellStyle name="Note 9" xfId="319"/>
+    <cellStyle name="Note 10" xfId="312"/>
+    <cellStyle name="Note 2" xfId="72"/>
+    <cellStyle name="Note 2 2" xfId="73"/>
+    <cellStyle name="Note 2 3" xfId="313"/>
+    <cellStyle name="Note 3" xfId="74"/>
+    <cellStyle name="Note 4" xfId="75"/>
+    <cellStyle name="Note 5" xfId="76"/>
+    <cellStyle name="Note 6" xfId="314"/>
+    <cellStyle name="Note 6 2" xfId="315"/>
+    <cellStyle name="Note 7" xfId="316"/>
+    <cellStyle name="Note 8" xfId="317"/>
+    <cellStyle name="Note 9" xfId="318"/>
     <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Output 2" xfId="78"/>
-    <cellStyle name="Output 2 2" xfId="79"/>
-    <cellStyle name="Output 2 3" xfId="321"/>
-    <cellStyle name="Output 3" xfId="80"/>
-    <cellStyle name="Output 4" xfId="81"/>
-    <cellStyle name="Output 5" xfId="322"/>
-    <cellStyle name="Output 5 2" xfId="323"/>
-    <cellStyle name="Output 6" xfId="324"/>
-    <cellStyle name="Output 7" xfId="325"/>
-    <cellStyle name="Output 8" xfId="326"/>
-    <cellStyle name="Output 9" xfId="320"/>
-    <cellStyle name="Percent 2" xfId="327"/>
+    <cellStyle name="Output 2" xfId="77"/>
+    <cellStyle name="Output 2 2" xfId="78"/>
+    <cellStyle name="Output 2 3" xfId="320"/>
+    <cellStyle name="Output 3" xfId="79"/>
+    <cellStyle name="Output 4" xfId="80"/>
+    <cellStyle name="Output 5" xfId="321"/>
+    <cellStyle name="Output 5 2" xfId="322"/>
+    <cellStyle name="Output 6" xfId="323"/>
+    <cellStyle name="Output 7" xfId="324"/>
+    <cellStyle name="Output 8" xfId="325"/>
+    <cellStyle name="Output 9" xfId="319"/>
+    <cellStyle name="Percent 2" xfId="326"/>
     <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Title 2" xfId="82"/>
-    <cellStyle name="Title 2 2" xfId="83"/>
-    <cellStyle name="Title 2 3" xfId="328"/>
-    <cellStyle name="Title 3" xfId="84"/>
-    <cellStyle name="Title 4" xfId="85"/>
-    <cellStyle name="Title 5" xfId="329"/>
-    <cellStyle name="Title 5 2" xfId="330"/>
-    <cellStyle name="Title 6" xfId="331"/>
+    <cellStyle name="Title 2" xfId="81"/>
+    <cellStyle name="Title 2 2" xfId="82"/>
+    <cellStyle name="Title 2 3" xfId="327"/>
+    <cellStyle name="Title 3" xfId="83"/>
+    <cellStyle name="Title 4" xfId="84"/>
+    <cellStyle name="Title 5" xfId="328"/>
+    <cellStyle name="Title 5 2" xfId="329"/>
+    <cellStyle name="Title 6" xfId="330"/>
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Total 2" xfId="86"/>
-    <cellStyle name="Total 2 2" xfId="87"/>
-    <cellStyle name="Total 2 3" xfId="333"/>
-    <cellStyle name="Total 3" xfId="88"/>
-    <cellStyle name="Total 4" xfId="89"/>
-    <cellStyle name="Total 5" xfId="334"/>
-    <cellStyle name="Total 5 2" xfId="335"/>
-    <cellStyle name="Total 6" xfId="336"/>
-    <cellStyle name="Total 7" xfId="337"/>
-    <cellStyle name="Total 8" xfId="338"/>
-    <cellStyle name="Total 9" xfId="332"/>
+    <cellStyle name="Total 2" xfId="85"/>
+    <cellStyle name="Total 2 2" xfId="86"/>
+    <cellStyle name="Total 2 3" xfId="332"/>
+    <cellStyle name="Total 3" xfId="87"/>
+    <cellStyle name="Total 4" xfId="88"/>
+    <cellStyle name="Total 5" xfId="333"/>
+    <cellStyle name="Total 5 2" xfId="334"/>
+    <cellStyle name="Total 6" xfId="335"/>
+    <cellStyle name="Total 7" xfId="336"/>
+    <cellStyle name="Total 8" xfId="337"/>
+    <cellStyle name="Total 9" xfId="331"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Warning Text 2" xfId="90"/>
-    <cellStyle name="Warning Text 2 2" xfId="91"/>
-    <cellStyle name="Warning Text 2 3" xfId="340"/>
-    <cellStyle name="Warning Text 3" xfId="92"/>
-    <cellStyle name="Warning Text 4" xfId="93"/>
-    <cellStyle name="Warning Text 5" xfId="341"/>
-    <cellStyle name="Warning Text 5 2" xfId="342"/>
-    <cellStyle name="Warning Text 6" xfId="343"/>
-    <cellStyle name="Warning Text 7" xfId="344"/>
-    <cellStyle name="Warning Text 8" xfId="345"/>
-    <cellStyle name="Warning Text 9" xfId="339"/>
+    <cellStyle name="Warning Text 2" xfId="89"/>
+    <cellStyle name="Warning Text 2 2" xfId="90"/>
+    <cellStyle name="Warning Text 2 3" xfId="339"/>
+    <cellStyle name="Warning Text 3" xfId="91"/>
+    <cellStyle name="Warning Text 4" xfId="92"/>
+    <cellStyle name="Warning Text 5" xfId="340"/>
+    <cellStyle name="Warning Text 5 2" xfId="341"/>
+    <cellStyle name="Warning Text 6" xfId="342"/>
+    <cellStyle name="Warning Text 7" xfId="343"/>
+    <cellStyle name="Warning Text 8" xfId="344"/>
+    <cellStyle name="Warning Text 9" xfId="338"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -6274,13 +6284,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6331,24 +6341,26 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3048000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1066800</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Creative Commons License">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6362,8 +6374,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609600" y="0"/>
-          <a:ext cx="3876675" cy="1066800"/>
+          <a:off x="609600" y="9048750"/>
+          <a:ext cx="838200" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10095,10 +10107,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:E42"/>
+  <dimension ref="B2:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10109,213 +10121,226 @@
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="102" customHeight="1"/>
-    <row r="3" spans="2:5" ht="18.75">
+    <row r="2" spans="2:5" ht="18.75">
+      <c r="B2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="117" t="s">
+        <v>415</v>
+      </c>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+    </row>
+    <row r="3" spans="2:5">
       <c r="B3" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="117" t="s">
-        <v>415</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>360</v>
       </c>
       <c r="D3" s="73"/>
       <c r="E3" s="73"/>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" ht="150">
       <c r="B4" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="76" t="s">
-        <v>360</v>
+        <v>2</v>
+      </c>
+      <c r="C4" s="113" t="s">
+        <v>419</v>
       </c>
       <c r="D4" s="73"/>
       <c r="E4" s="73"/>
     </row>
-    <row r="5" spans="2:5" ht="150">
+    <row r="5" spans="2:5" ht="30">
       <c r="B5" s="74" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="113" t="s">
-        <v>419</v>
+        <v>3</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>412</v>
       </c>
       <c r="D5" s="73"/>
       <c r="E5" s="73"/>
     </row>
-    <row r="6" spans="2:5" ht="30">
-      <c r="B6" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="75" t="s">
-        <v>412</v>
-      </c>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
+    <row r="8" spans="2:5">
+      <c r="B8" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="68" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="68" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="68" t="s">
-        <v>6</v>
+      <c r="B9" s="66">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="67">
+        <v>40409</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="66">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D10" s="70" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="67">
-        <v>40409</v>
+        <v>40413</v>
       </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="66">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>83</v>
+        <v>193</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="E11" s="67">
-        <v>40413</v>
+        <v>40441</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="66">
-        <v>0.3</v>
+      <c r="B12" s="66" t="s">
+        <v>194</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D12" s="70" t="s">
         <v>190</v>
       </c>
       <c r="E12" s="67">
-        <v>40441</v>
+        <v>40478</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="66" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>195</v>
+        <v>259</v>
       </c>
       <c r="D13" s="70" t="s">
         <v>190</v>
       </c>
       <c r="E13" s="67">
-        <v>40478</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
+        <v>40487</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="30">
       <c r="B14" s="66" t="s">
         <v>214</v>
       </c>
-      <c r="C14" s="63" t="s">
-        <v>259</v>
-      </c>
-      <c r="D14" s="70" t="s">
+      <c r="C14" s="65" t="s">
+        <v>256</v>
+      </c>
+      <c r="D14" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="E14" s="67">
-        <v>40487</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="30">
+      <c r="E14" s="64">
+        <v>40500</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
       <c r="B15" s="66" t="s">
         <v>214</v>
       </c>
-      <c r="C15" s="65" t="s">
-        <v>256</v>
-      </c>
-      <c r="D15" s="72" t="s">
+      <c r="C15" s="63" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" s="70" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="64">
-        <v>40500</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
+      <c r="E15" s="67">
+        <v>40505</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="30">
       <c r="B16" s="66" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="D16" s="70" t="s">
         <v>190</v>
       </c>
       <c r="E16" s="67">
-        <v>40505</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="30">
+        <v>40506</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
       <c r="B17" s="66" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D17" s="70" t="s">
         <v>190</v>
       </c>
       <c r="E17" s="67">
-        <v>40506</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="66" t="s">
-        <v>268</v>
-      </c>
-      <c r="C18" s="63" t="s">
-        <v>270</v>
-      </c>
-      <c r="D18" s="70" t="s">
+        <v>40512</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30">
+      <c r="B18" s="62" t="s">
+        <v>271</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>352</v>
+      </c>
+      <c r="D18" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="E18" s="67">
-        <v>40512</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="30">
-      <c r="B19" s="62" t="s">
-        <v>271</v>
+      <c r="E18" s="60">
+        <v>40557</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="60">
+      <c r="B19" s="59" t="s">
+        <v>288</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>352</v>
-      </c>
-      <c r="D19" s="61" t="s">
+        <v>353</v>
+      </c>
+      <c r="D19" s="65" t="s">
         <v>190</v>
       </c>
-      <c r="E19" s="60">
-        <v>40557</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="60">
-      <c r="B20" s="59" t="s">
+      <c r="E19" s="58">
+        <v>40590</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="66" t="s">
         <v>288</v>
       </c>
-      <c r="C20" s="65" t="s">
-        <v>353</v>
-      </c>
-      <c r="D20" s="65" t="s">
+      <c r="C20" s="63" t="s">
+        <v>318</v>
+      </c>
+      <c r="D20" s="70" t="s">
         <v>190</v>
       </c>
-      <c r="E20" s="58">
-        <v>40590</v>
+      <c r="E20" s="67">
+        <v>40612</v>
       </c>
     </row>
     <row r="21" spans="2:5">
@@ -10332,192 +10357,183 @@
         <v>40612</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" ht="30">
       <c r="B22" s="66" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D22" s="70" t="s">
         <v>190</v>
       </c>
       <c r="E22" s="67">
-        <v>40612</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="30">
+        <v>40690</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" s="66" t="s">
         <v>319</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="D23" s="70" t="s">
-        <v>190</v>
+        <v>326</v>
       </c>
       <c r="E23" s="67">
-        <v>40690</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
+        <v>40694</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="45">
       <c r="B24" s="66" t="s">
         <v>319</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D24" s="70" t="s">
-        <v>326</v>
+        <v>190</v>
       </c>
       <c r="E24" s="67">
-        <v>40694</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="45">
+        <v>40698</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" s="66" t="s">
-        <v>319</v>
+        <v>349</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>327</v>
+        <v>348</v>
       </c>
       <c r="D25" s="70" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="E25" s="67">
-        <v>40698</v>
+        <v>40760</v>
       </c>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="66" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="D26" s="70" t="s">
         <v>347</v>
       </c>
       <c r="E26" s="67">
-        <v>40760</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
+        <v>40767</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="30">
       <c r="B27" s="66" t="s">
         <v>360</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>361</v>
-      </c>
-      <c r="D27" s="70" t="s">
-        <v>347</v>
-      </c>
-      <c r="E27" s="67">
-        <v>40767</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="30">
+        <v>366</v>
+      </c>
+      <c r="D27" s="74" t="s">
+        <v>367</v>
+      </c>
+      <c r="E27" s="64">
+        <v>40773</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" s="79" customFormat="1" ht="30">
       <c r="B28" s="66" t="s">
         <v>360</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>366</v>
-      </c>
-      <c r="D28" s="74" t="s">
-        <v>367</v>
-      </c>
-      <c r="E28" s="64">
-        <v>40773</v>
+        <v>411</v>
+      </c>
+      <c r="D28" s="70" t="s">
+        <v>190</v>
+      </c>
+      <c r="E28" s="67">
+        <v>40781</v>
       </c>
     </row>
     <row r="29" spans="2:5" s="79" customFormat="1" ht="30">
       <c r="B29" s="66" t="s">
-        <v>360</v>
+        <v>413</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D29" s="70" t="s">
         <v>190</v>
       </c>
       <c r="E29" s="67">
-        <v>40781</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" s="79" customFormat="1" ht="30">
-      <c r="B30" s="66" t="s">
-        <v>413</v>
-      </c>
-      <c r="C30" s="63" t="s">
-        <v>414</v>
-      </c>
-      <c r="D30" s="70" t="s">
-        <v>190</v>
-      </c>
-      <c r="E30" s="67">
         <v>40970</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="79" customFormat="1">
+    <row r="30" spans="2:5" s="79" customFormat="1">
+      <c r="B30" s="66"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="67"/>
+    </row>
+    <row r="31" spans="2:5">
       <c r="B31" s="66"/>
       <c r="C31" s="63"/>
       <c r="D31" s="70"/>
       <c r="E31" s="67"/>
     </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="66"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="67"/>
-    </row>
-    <row r="33" spans="2:5" ht="15.75" thickBot="1"/>
-    <row r="34" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B34" s="123"/>
-      <c r="C34" s="124" t="s">
+    <row r="32" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="33" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B33" s="123"/>
+      <c r="C33" s="208" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="18" thickBot="1">
-      <c r="C37" s="149" t="s">
+    <row r="34" spans="2:5">
+      <c r="C34" s="209" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="18" thickBot="1">
+      <c r="C36" s="148" t="s">
         <v>430</v>
       </c>
-      <c r="D37" s="152"/>
-      <c r="E37" s="152"/>
-    </row>
-    <row r="38" spans="2:5" ht="15.75" thickTop="1">
-      <c r="C38" s="148" t="s">
+      <c r="D36" s="151"/>
+      <c r="E36" s="151"/>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" thickTop="1">
+      <c r="C37" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="147" t="s">
+      <c r="D37" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="147" t="s">
+      <c r="E37" s="146" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="38" spans="2:5">
+      <c r="C38" s="152"/>
+      <c r="D38" s="150"/>
+      <c r="E38" s="149"/>
+    </row>
     <row r="39" spans="2:5">
-      <c r="C39" s="153"/>
-      <c r="D39" s="151"/>
-      <c r="E39" s="150"/>
+      <c r="C39" s="152"/>
+      <c r="D39" s="150"/>
+      <c r="E39" s="152"/>
     </row>
     <row r="40" spans="2:5">
-      <c r="C40" s="153"/>
-      <c r="D40" s="151"/>
-      <c r="E40" s="153"/>
+      <c r="C40" s="152"/>
+      <c r="D40" s="150"/>
+      <c r="E40" s="152"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="C41" s="153"/>
-      <c r="D41" s="151"/>
-      <c r="E41" s="153"/>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="C42" s="153"/>
-      <c r="D42" s="151"/>
-      <c r="E42" s="153"/>
+      <c r="C41" s="152"/>
+      <c r="D41" s="150"/>
+      <c r="E41" s="152"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C34" r:id="rId1" display="http://creativecommons.org/licenses/by/3.0/"/>
+    <hyperlink ref="C33" r:id="rId1" display="http://creativecommons.org/licenses/by/3.0/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -10789,20 +10805,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="173" t="s">
         <v>364</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="172" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="173"/>
+      <c r="B2" s="172"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1">
       <c r="A3" t="s">
@@ -10911,294 +10927,294 @@
   </sheetPr>
   <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" style="165" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="165"/>
-    <col min="3" max="3" width="17.140625" style="169"/>
-    <col min="4" max="18" width="17.140625" style="165"/>
-    <col min="19" max="19" width="49" style="165" customWidth="1"/>
-    <col min="20" max="28" width="17.140625" style="165"/>
-    <col min="29" max="30" width="17.140625" style="169"/>
-    <col min="31" max="16384" width="17.140625" style="165"/>
+    <col min="1" max="1" width="38.7109375" style="164" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="164"/>
+    <col min="3" max="3" width="17.140625" style="168"/>
+    <col min="4" max="18" width="17.140625" style="164"/>
+    <col min="19" max="19" width="49" style="164" customWidth="1"/>
+    <col min="20" max="28" width="17.140625" style="164"/>
+    <col min="29" max="30" width="17.140625" style="168"/>
+    <col min="31" max="16384" width="17.140625" style="164"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="18" customHeight="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="175" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="177" t="s">
+      <c r="B1" s="175"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="176" t="s">
         <v>265</v>
       </c>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="H1" s="178" t="s">
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="H1" s="177" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="177" t="s">
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="176" t="s">
         <v>201</v>
       </c>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="160" t="s">
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
+      <c r="O1" s="176"/>
+      <c r="P1" s="176"/>
+      <c r="Q1" s="176"/>
+      <c r="R1" s="176"/>
+      <c r="S1" s="176"/>
+      <c r="T1" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="161"/>
-      <c r="V1" s="161"/>
-      <c r="W1" s="161"/>
-      <c r="X1" s="171" t="s">
+      <c r="U1" s="160"/>
+      <c r="V1" s="160"/>
+      <c r="W1" s="160"/>
+      <c r="X1" s="170" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="167"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="166"/>
-      <c r="AB1" s="166"/>
-      <c r="AC1" s="179" t="s">
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="165"/>
+      <c r="AA1" s="165"/>
+      <c r="AB1" s="165"/>
+      <c r="AC1" s="178" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="179"/>
-      <c r="AE1" s="163" t="s">
+      <c r="AD1" s="178"/>
+      <c r="AE1" s="162" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" s="172"/>
-      <c r="AG1" s="172"/>
-      <c r="AH1" s="172"/>
-      <c r="AI1" s="172"/>
-      <c r="AJ1" s="172"/>
-      <c r="AK1" s="172"/>
-      <c r="AL1" s="175" t="s">
+      <c r="AF1" s="171"/>
+      <c r="AG1" s="171"/>
+      <c r="AH1" s="171"/>
+      <c r="AI1" s="171"/>
+      <c r="AJ1" s="171"/>
+      <c r="AK1" s="171"/>
+      <c r="AL1" s="174" t="s">
         <v>55</v>
       </c>
-      <c r="AM1" s="175"/>
-      <c r="AN1" s="175"/>
-      <c r="AO1" s="175"/>
-      <c r="AP1" s="175"/>
-      <c r="AQ1" s="175"/>
-      <c r="AR1" s="175"/>
-      <c r="AS1" s="175"/>
-      <c r="AT1" s="175"/>
-      <c r="AU1" s="175"/>
-      <c r="AV1" s="175"/>
-      <c r="AW1" s="168"/>
-      <c r="AX1" s="159"/>
-      <c r="AY1" s="159"/>
-      <c r="AZ1" s="162" t="s">
+      <c r="AM1" s="174"/>
+      <c r="AN1" s="174"/>
+      <c r="AO1" s="174"/>
+      <c r="AP1" s="174"/>
+      <c r="AQ1" s="174"/>
+      <c r="AR1" s="174"/>
+      <c r="AS1" s="174"/>
+      <c r="AT1" s="174"/>
+      <c r="AU1" s="174"/>
+      <c r="AV1" s="174"/>
+      <c r="AW1" s="167"/>
+      <c r="AX1" s="158"/>
+      <c r="AY1" s="158"/>
+      <c r="AZ1" s="161" t="s">
         <v>67</v>
       </c>
-      <c r="BA1" s="162"/>
-      <c r="BB1" s="162"/>
-      <c r="BC1" s="162"/>
-      <c r="BD1" s="162"/>
-      <c r="BE1" s="162"/>
-      <c r="BF1" s="162"/>
-      <c r="BG1" s="162"/>
-      <c r="BH1" s="162"/>
-      <c r="BI1" s="162"/>
-      <c r="BJ1" s="162"/>
-      <c r="BK1" s="159"/>
-    </row>
-    <row r="2" spans="1:63" s="164" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A2" s="154" t="s">
+      <c r="BA1" s="161"/>
+      <c r="BB1" s="161"/>
+      <c r="BC1" s="161"/>
+      <c r="BD1" s="161"/>
+      <c r="BE1" s="161"/>
+      <c r="BF1" s="161"/>
+      <c r="BG1" s="161"/>
+      <c r="BH1" s="161"/>
+      <c r="BI1" s="161"/>
+      <c r="BJ1" s="161"/>
+      <c r="BK1" s="158"/>
+    </row>
+    <row r="2" spans="1:63" s="163" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A2" s="153" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="153" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="155" t="s">
+      <c r="C2" s="154" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="154" t="s">
+      <c r="D2" s="153" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="154" t="s">
+      <c r="E2" s="153" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="154" t="s">
+      <c r="F2" s="153" t="s">
         <v>199</v>
       </c>
-      <c r="G2" s="154" t="s">
+      <c r="G2" s="153" t="s">
         <v>191</v>
       </c>
-      <c r="H2" s="154" t="s">
+      <c r="H2" s="153" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="154" t="s">
+      <c r="I2" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="154" t="s">
+      <c r="J2" s="153" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="154" t="s">
+      <c r="K2" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="154" t="s">
+      <c r="L2" s="153" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="154" t="s">
+      <c r="M2" s="153" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="154" t="s">
+      <c r="N2" s="153" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="156" t="s">
+      <c r="O2" s="155" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="154" t="s">
+      <c r="P2" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="154" t="s">
+      <c r="Q2" s="153" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="154" t="s">
+      <c r="R2" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="154" t="s">
+      <c r="S2" s="153" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="157" t="s">
+      <c r="T2" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="154" t="s">
+      <c r="U2" s="153" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="154" t="s">
+      <c r="V2" s="153" t="s">
         <v>81</v>
       </c>
-      <c r="W2" s="157" t="s">
+      <c r="W2" s="156" t="s">
         <v>82</v>
       </c>
-      <c r="X2" s="157" t="s">
+      <c r="X2" s="156" t="s">
         <v>287</v>
       </c>
-      <c r="Y2" s="154" t="s">
+      <c r="Y2" s="153" t="s">
         <v>188</v>
       </c>
-      <c r="Z2" s="154" t="s">
+      <c r="Z2" s="153" t="s">
         <v>286</v>
       </c>
-      <c r="AA2" s="154" t="s">
+      <c r="AA2" s="153" t="s">
         <v>285</v>
       </c>
-      <c r="AB2" s="154" t="s">
+      <c r="AB2" s="153" t="s">
         <v>189</v>
       </c>
-      <c r="AC2" s="155" t="s">
+      <c r="AC2" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="AD2" s="155" t="s">
+      <c r="AD2" s="154" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" s="154" t="s">
+      <c r="AE2" s="153" t="s">
         <v>84</v>
       </c>
-      <c r="AF2" s="154" t="s">
+      <c r="AF2" s="153" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="154" t="s">
+      <c r="AG2" s="153" t="s">
         <v>50</v>
       </c>
-      <c r="AH2" s="154" t="s">
+      <c r="AH2" s="153" t="s">
         <v>52</v>
       </c>
-      <c r="AI2" s="154" t="s">
+      <c r="AI2" s="153" t="s">
         <v>51</v>
       </c>
-      <c r="AJ2" s="154" t="s">
+      <c r="AJ2" s="153" t="s">
         <v>53</v>
       </c>
-      <c r="AK2" s="154" t="s">
+      <c r="AK2" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="AL2" s="154" t="s">
+      <c r="AL2" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="AM2" s="154" t="s">
+      <c r="AM2" s="153" t="s">
         <v>57</v>
       </c>
-      <c r="AN2" s="154" t="s">
+      <c r="AN2" s="153" t="s">
         <v>267</v>
       </c>
-      <c r="AO2" s="154" t="s">
+      <c r="AO2" s="153" t="s">
         <v>58</v>
       </c>
-      <c r="AP2" s="154" t="s">
+      <c r="AP2" s="153" t="s">
         <v>59</v>
       </c>
-      <c r="AQ2" s="154" t="s">
+      <c r="AQ2" s="153" t="s">
         <v>60</v>
       </c>
-      <c r="AR2" s="154" t="s">
+      <c r="AR2" s="153" t="s">
         <v>61</v>
       </c>
-      <c r="AS2" s="154" t="s">
+      <c r="AS2" s="153" t="s">
         <v>62</v>
       </c>
-      <c r="AT2" s="154" t="s">
+      <c r="AT2" s="153" t="s">
         <v>63</v>
       </c>
-      <c r="AU2" s="154" t="s">
+      <c r="AU2" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="AV2" s="154" t="s">
+      <c r="AV2" s="153" t="s">
         <v>65</v>
       </c>
-      <c r="AW2" s="158" t="s">
+      <c r="AW2" s="157" t="s">
         <v>66</v>
       </c>
-      <c r="AX2" s="154" t="s">
+      <c r="AX2" s="153" t="s">
         <v>78</v>
       </c>
-      <c r="AY2" s="154" t="s">
+      <c r="AY2" s="153" t="s">
         <v>85</v>
       </c>
-      <c r="AZ2" s="154" t="s">
+      <c r="AZ2" s="153" t="s">
         <v>261</v>
       </c>
-      <c r="BA2" s="154" t="s">
+      <c r="BA2" s="153" t="s">
         <v>68</v>
       </c>
-      <c r="BB2" s="154" t="s">
+      <c r="BB2" s="153" t="s">
         <v>266</v>
       </c>
-      <c r="BC2" s="154" t="s">
+      <c r="BC2" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="BD2" s="154" t="s">
+      <c r="BD2" s="153" t="s">
         <v>69</v>
       </c>
-      <c r="BE2" s="154" t="s">
+      <c r="BE2" s="153" t="s">
         <v>70</v>
       </c>
-      <c r="BF2" s="154" t="s">
+      <c r="BF2" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="BG2" s="154" t="s">
+      <c r="BG2" s="153" t="s">
         <v>72</v>
       </c>
-      <c r="BH2" s="154" t="s">
+      <c r="BH2" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="BI2" s="154" t="s">
+      <c r="BI2" s="153" t="s">
         <v>75</v>
       </c>
-      <c r="BJ2" s="154" t="s">
+      <c r="BJ2" s="153" t="s">
         <v>76</v>
       </c>
-      <c r="BK2" s="154" t="s">
+      <c r="BK2" s="153" t="s">
         <v>272</v>
       </c>
     </row>
@@ -11259,457 +11275,457 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.9" customHeight="1">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="128" t="s">
         <v>421</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
     </row>
     <row r="2" spans="1:9" ht="18.75">
-      <c r="A2" s="132"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
+      <c r="A2" s="131"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
     </row>
     <row r="3" spans="1:9" ht="36" customHeight="1">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="180" t="s">
         <v>422</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
+      <c r="B3" s="180"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
     </row>
     <row r="4" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A4" s="132"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="142"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
+      <c r="A4" s="131"/>
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="126"/>
     </row>
     <row r="5" spans="1:9" ht="72" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="185" t="s">
+      <c r="A5" s="184" t="s">
         <v>423</v>
       </c>
-      <c r="B5" s="186"/>
-      <c r="C5" s="186"/>
-      <c r="D5" s="186"/>
-      <c r="E5" s="186"/>
-      <c r="F5" s="186"/>
-      <c r="G5" s="187"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
+      <c r="B5" s="185"/>
+      <c r="C5" s="185"/>
+      <c r="D5" s="185"/>
+      <c r="E5" s="185"/>
+      <c r="F5" s="185"/>
+      <c r="G5" s="186"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A6" s="127"/>
-      <c r="B6" s="127"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
+      <c r="A6" s="126"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
     </row>
     <row r="7" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A7" s="182" t="s">
+      <c r="A7" s="181" t="s">
         <v>424</v>
       </c>
-      <c r="B7" s="183"/>
-      <c r="C7" s="183"/>
-      <c r="D7" s="184"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
+      <c r="B7" s="182"/>
+      <c r="C7" s="182"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A8" s="127"/>
-      <c r="B8" s="127"/>
-      <c r="C8" s="127"/>
-      <c r="D8" s="127"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
+      <c r="A8" s="126"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="126"/>
     </row>
     <row r="9" spans="1:9" ht="18.75">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="131" t="s">
         <v>321</v>
       </c>
-      <c r="B9" s="127"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="142"/>
-      <c r="E9" s="127"/>
-      <c r="F9" s="127"/>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="127"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A10" s="180"/>
-      <c r="B10" s="180"/>
-      <c r="C10" s="180"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="127"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="127"/>
+      <c r="A10" s="179"/>
+      <c r="B10" s="179"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="126"/>
+      <c r="I10" s="126"/>
     </row>
     <row r="11" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A11" s="141" t="s">
+      <c r="A11" s="140" t="s">
         <v>322</v>
       </c>
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="140" t="s">
         <v>323</v>
       </c>
-      <c r="C11" s="141" t="s">
+      <c r="C11" s="140" t="s">
         <v>324</v>
       </c>
-      <c r="D11" s="141" t="s">
+      <c r="D11" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="141" t="s">
+      <c r="E11" s="140" t="s">
         <v>354</v>
       </c>
-      <c r="F11" s="144" t="s">
+      <c r="F11" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="141" t="s">
+      <c r="G11" s="140" t="s">
         <v>351</v>
       </c>
-      <c r="H11" s="141" t="s">
+      <c r="H11" s="140" t="s">
         <v>425</v>
       </c>
-      <c r="I11" s="141" t="s">
+      <c r="I11" s="140" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="140"/>
-      <c r="B12" s="140"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="140"/>
+      <c r="A12" s="139"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
     </row>
     <row r="13" spans="1:9" ht="30">
-      <c r="A13" s="140"/>
-      <c r="B13" s="140"/>
-      <c r="C13" s="140"/>
-      <c r="D13" s="137" t="s">
+      <c r="A13" s="139"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="136" t="s">
         <v>426</v>
       </c>
-      <c r="E13" s="137" t="s">
+      <c r="E13" s="136" t="s">
         <v>362</v>
       </c>
-      <c r="F13" s="136">
+      <c r="F13" s="135">
         <v>40766</v>
       </c>
-      <c r="G13" s="135" t="s">
+      <c r="G13" s="134" t="s">
         <v>427</v>
       </c>
-      <c r="H13" s="137" t="s">
+      <c r="H13" s="136" t="s">
         <v>363</v>
       </c>
-      <c r="I13" s="136">
+      <c r="I13" s="135">
         <v>40770</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45">
-      <c r="A14" s="140"/>
-      <c r="B14" s="138"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="137" t="s">
+      <c r="A14" s="139"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="136" t="s">
         <v>428</v>
       </c>
-      <c r="E14" s="137"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="137"/>
-      <c r="H14" s="137"/>
-      <c r="I14" s="136"/>
+      <c r="E14" s="136"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="136"/>
+      <c r="H14" s="136"/>
+      <c r="I14" s="135"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="140"/>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="140"/>
-      <c r="F15" s="139"/>
-      <c r="G15" s="140"/>
-      <c r="H15" s="140"/>
-      <c r="I15" s="140"/>
+      <c r="A15" s="139"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="137"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="138"/>
+      <c r="G15" s="139"/>
+      <c r="H15" s="139"/>
+      <c r="I15" s="139"/>
     </row>
     <row r="16" spans="1:9" ht="90">
-      <c r="A16" s="140"/>
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="146" t="s">
+      <c r="A16" s="139"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="137"/>
+      <c r="D16" s="145" t="s">
         <v>429</v>
       </c>
-      <c r="E16" s="140"/>
-      <c r="F16" s="139"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="140"/>
-      <c r="I16" s="140"/>
+      <c r="E16" s="139"/>
+      <c r="F16" s="138"/>
+      <c r="G16" s="139"/>
+      <c r="H16" s="139"/>
+      <c r="I16" s="139"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="140"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="139"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="140"/>
-      <c r="I17" s="140"/>
+      <c r="A17" s="139"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="139"/>
+      <c r="H17" s="139"/>
+      <c r="I17" s="139"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="140"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="139"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="140"/>
-      <c r="I18" s="140"/>
+      <c r="A18" s="139"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="139"/>
+      <c r="H18" s="139"/>
+      <c r="I18" s="139"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="140"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="139"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="140"/>
-      <c r="I19" s="140"/>
+      <c r="A19" s="139"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="139"/>
+      <c r="I19" s="139"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="140"/>
-      <c r="B20" s="138"/>
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
-      <c r="E20" s="140"/>
-      <c r="F20" s="139"/>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140"/>
-      <c r="I20" s="140"/>
+      <c r="A20" s="139"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="139"/>
+      <c r="I20" s="139"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="140"/>
-      <c r="B21" s="138"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="145"/>
-      <c r="E21" s="140"/>
-      <c r="F21" s="133"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="140"/>
-      <c r="I21" s="140"/>
+      <c r="A21" s="139"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="144"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="132"/>
+      <c r="G21" s="139"/>
+      <c r="H21" s="139"/>
+      <c r="I21" s="139"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="128"/>
-      <c r="B22" s="138"/>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="128"/>
-      <c r="H22" s="140"/>
-      <c r="I22" s="140"/>
+      <c r="A22" s="127"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="132"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="139"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="140"/>
-      <c r="B23" s="138"/>
-      <c r="C23" s="138"/>
-      <c r="D23" s="145"/>
-      <c r="E23" s="140"/>
-      <c r="F23" s="133"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="140"/>
+      <c r="A23" s="139"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="132"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="139"/>
+      <c r="I23" s="139"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="140"/>
-      <c r="B24" s="138"/>
-      <c r="C24" s="138"/>
-      <c r="D24" s="126"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="140"/>
-      <c r="H24" s="140"/>
-      <c r="I24" s="140"/>
+      <c r="A24" s="139"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="132"/>
+      <c r="G24" s="139"/>
+      <c r="H24" s="139"/>
+      <c r="I24" s="139"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="140"/>
-      <c r="B25" s="138"/>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="140"/>
-      <c r="F25" s="139"/>
-      <c r="G25" s="140"/>
-      <c r="H25" s="140"/>
-      <c r="I25" s="140"/>
+      <c r="A25" s="139"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="139"/>
+      <c r="H25" s="139"/>
+      <c r="I25" s="139"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="140"/>
-      <c r="B26" s="138"/>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="133"/>
-      <c r="G26" s="140"/>
-      <c r="H26" s="140"/>
-      <c r="I26" s="140"/>
+      <c r="A26" s="139"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="137"/>
+      <c r="D26" s="137"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="132"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="139"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="140"/>
-      <c r="B27" s="138"/>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="139"/>
-      <c r="G27" s="140"/>
-      <c r="H27" s="140"/>
-      <c r="I27" s="140"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="137"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="138"/>
+      <c r="G27" s="139"/>
+      <c r="H27" s="139"/>
+      <c r="I27" s="139"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="140"/>
-      <c r="B28" s="138"/>
-      <c r="C28" s="138"/>
-      <c r="D28" s="138"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="140"/>
-      <c r="H28" s="140"/>
-      <c r="I28" s="140"/>
+      <c r="A28" s="139"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="138"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="139"/>
+      <c r="I28" s="139"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="140"/>
-      <c r="B29" s="138"/>
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="139"/>
-      <c r="G29" s="140"/>
-      <c r="H29" s="140"/>
-      <c r="I29" s="140"/>
+      <c r="A29" s="139"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="137"/>
+      <c r="D29" s="137"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="138"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="139"/>
+      <c r="I29" s="139"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="140"/>
-      <c r="B30" s="138"/>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="139"/>
-      <c r="G30" s="140"/>
-      <c r="H30" s="140"/>
-      <c r="I30" s="140"/>
+      <c r="A30" s="139"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="137"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="138"/>
+      <c r="G30" s="139"/>
+      <c r="H30" s="139"/>
+      <c r="I30" s="139"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="143"/>
-      <c r="B31" s="143"/>
-      <c r="C31" s="143"/>
-      <c r="D31" s="143"/>
-      <c r="E31" s="143"/>
-      <c r="F31" s="130"/>
-      <c r="G31" s="143"/>
-      <c r="H31" s="143"/>
-      <c r="I31" s="143"/>
+      <c r="A31" s="142"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="142"/>
+      <c r="I31" s="142"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="127"/>
-      <c r="B32" s="127"/>
-      <c r="C32" s="127"/>
-      <c r="D32" s="127"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="127"/>
-      <c r="G32" s="127"/>
-      <c r="H32" s="127"/>
-      <c r="I32" s="127"/>
+      <c r="A32" s="126"/>
+      <c r="B32" s="126"/>
+      <c r="C32" s="126"/>
+      <c r="D32" s="126"/>
+      <c r="E32" s="126"/>
+      <c r="F32" s="126"/>
+      <c r="G32" s="126"/>
+      <c r="H32" s="126"/>
+      <c r="I32" s="126"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="127"/>
-      <c r="B33" s="127"/>
-      <c r="C33" s="127"/>
-      <c r="D33" s="127"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="127"/>
-      <c r="G33" s="127"/>
-      <c r="H33" s="127"/>
-      <c r="I33" s="127"/>
+      <c r="A33" s="126"/>
+      <c r="B33" s="126"/>
+      <c r="C33" s="126"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="126"/>
+      <c r="G33" s="126"/>
+      <c r="H33" s="126"/>
+      <c r="I33" s="126"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="127"/>
-      <c r="B34" s="127"/>
-      <c r="C34" s="127"/>
-      <c r="D34" s="127"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="127"/>
-      <c r="G34" s="127"/>
-      <c r="H34" s="127"/>
-      <c r="I34" s="127"/>
+      <c r="A34" s="126"/>
+      <c r="B34" s="126"/>
+      <c r="C34" s="126"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="126"/>
+      <c r="F34" s="126"/>
+      <c r="G34" s="126"/>
+      <c r="H34" s="126"/>
+      <c r="I34" s="126"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="127"/>
-      <c r="B35" s="127"/>
-      <c r="C35" s="127"/>
-      <c r="D35" s="127"/>
-      <c r="E35" s="127"/>
-      <c r="F35" s="127"/>
-      <c r="G35" s="127"/>
-      <c r="H35" s="127"/>
-      <c r="I35" s="127"/>
+      <c r="A35" s="126"/>
+      <c r="B35" s="126"/>
+      <c r="C35" s="126"/>
+      <c r="D35" s="126"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="126"/>
+      <c r="G35" s="126"/>
+      <c r="H35" s="126"/>
+      <c r="I35" s="126"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="127"/>
-      <c r="B36" s="127"/>
-      <c r="C36" s="127"/>
-      <c r="D36" s="127"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="127"/>
-      <c r="G36" s="127"/>
-      <c r="H36" s="127"/>
-      <c r="I36" s="127"/>
+      <c r="A36" s="126"/>
+      <c r="B36" s="126"/>
+      <c r="C36" s="126"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="126"/>
+      <c r="F36" s="126"/>
+      <c r="G36" s="126"/>
+      <c r="H36" s="126"/>
+      <c r="I36" s="126"/>
     </row>
     <row r="37" spans="1:9" ht="18.75">
-      <c r="A37" s="132" t="s">
+      <c r="A37" s="131" t="s">
         <v>350</v>
       </c>
-      <c r="B37" s="127"/>
-      <c r="C37" s="127"/>
-      <c r="D37" s="127"/>
-      <c r="E37" s="127"/>
-      <c r="F37" s="127"/>
-      <c r="G37" s="127"/>
-      <c r="H37" s="127"/>
-      <c r="I37" s="127"/>
+      <c r="B37" s="126"/>
+      <c r="C37" s="126"/>
+      <c r="D37" s="126"/>
+      <c r="E37" s="126"/>
+      <c r="F37" s="126"/>
+      <c r="G37" s="126"/>
+      <c r="H37" s="126"/>
+      <c r="I37" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -11747,14 +11763,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="193" t="s">
         <v>365</v>
       </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
-      <c r="F1" s="195"/>
+      <c r="B1" s="193"/>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="194"/>
       <c r="H1" s="54"/>
       <c r="I1" s="55"/>
     </row>
@@ -11797,7 +11813,7 @@
       <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A4" s="196" t="s">
+      <c r="A4" s="195" t="s">
         <v>187</v>
       </c>
       <c r="B4" s="80" t="s">
@@ -11822,7 +11838,7 @@
       <c r="I4" s="55"/>
     </row>
     <row r="5" spans="1:9" ht="100.15" customHeight="1">
-      <c r="A5" s="197"/>
+      <c r="A5" s="196"/>
       <c r="B5" s="80" t="s">
         <v>26</v>
       </c>
@@ -11868,7 +11884,7 @@
       <c r="I6" s="55"/>
     </row>
     <row r="7" spans="1:9" ht="18.600000000000001" customHeight="1">
-      <c r="A7" s="198" t="s">
+      <c r="A7" s="197" t="s">
         <v>200</v>
       </c>
       <c r="B7" s="80" t="s">
@@ -11880,7 +11896,7 @@
       <c r="D7" s="95" t="s">
         <v>380</v>
       </c>
-      <c r="E7" s="202" t="s">
+      <c r="E7" s="201" t="s">
         <v>379</v>
       </c>
       <c r="F7" s="38" t="s">
@@ -11893,7 +11909,7 @@
       <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:9" ht="60">
-      <c r="A8" s="189"/>
+      <c r="A8" s="188"/>
       <c r="B8" s="80" t="s">
         <v>32</v>
       </c>
@@ -11903,7 +11919,7 @@
       <c r="D8" s="92" t="s">
         <v>380</v>
       </c>
-      <c r="E8" s="203"/>
+      <c r="E8" s="202"/>
       <c r="F8" s="38" t="s">
         <v>299</v>
       </c>
@@ -11914,7 +11930,7 @@
       <c r="I8" s="55"/>
     </row>
     <row r="9" spans="1:9" ht="60">
-      <c r="A9" s="189"/>
+      <c r="A9" s="188"/>
       <c r="B9" s="80" t="s">
         <v>199</v>
       </c>
@@ -11924,7 +11940,7 @@
       <c r="D9" s="98" t="s">
         <v>380</v>
       </c>
-      <c r="E9" s="204"/>
+      <c r="E9" s="203"/>
       <c r="F9" s="38" t="s">
         <v>300</v>
       </c>
@@ -11958,7 +11974,7 @@
       <c r="I10" s="55"/>
     </row>
     <row r="11" spans="1:9" ht="45">
-      <c r="A11" s="199" t="s">
+      <c r="A11" s="198" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="50" t="s">
@@ -11985,7 +12001,7 @@
       <c r="I11" s="55"/>
     </row>
     <row r="12" spans="1:9" ht="75">
-      <c r="A12" s="200"/>
+      <c r="A12" s="199"/>
       <c r="B12" s="50" t="s">
         <v>28</v>
       </c>
@@ -12010,7 +12026,7 @@
       <c r="I12" s="55"/>
     </row>
     <row r="13" spans="1:9" ht="34.15" customHeight="1">
-      <c r="A13" s="201"/>
+      <c r="A13" s="200"/>
       <c r="B13" s="50" t="s">
         <v>29</v>
       </c>
@@ -12035,7 +12051,7 @@
       <c r="I13" s="55"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="189" t="s">
+      <c r="A14" s="188" t="s">
         <v>201</v>
       </c>
       <c r="B14" s="50" t="s">
@@ -12060,7 +12076,7 @@
       <c r="I14" s="55"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="189"/>
+      <c r="A15" s="188"/>
       <c r="B15" s="50" t="s">
         <v>34</v>
       </c>
@@ -12083,7 +12099,7 @@
       <c r="I15" s="55"/>
     </row>
     <row r="16" spans="1:9" ht="22.5">
-      <c r="A16" s="189"/>
+      <c r="A16" s="188"/>
       <c r="B16" s="50" t="s">
         <v>35</v>
       </c>
@@ -12106,7 +12122,7 @@
       <c r="I16" s="55"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="189"/>
+      <c r="A17" s="188"/>
       <c r="B17" s="50" t="s">
         <v>36</v>
       </c>
@@ -12129,7 +12145,7 @@
       <c r="I17" s="55"/>
     </row>
     <row r="18" spans="1:9" ht="45">
-      <c r="A18" s="189"/>
+      <c r="A18" s="188"/>
       <c r="B18" s="35" t="s">
         <v>37</v>
       </c>
@@ -12139,7 +12155,7 @@
       <c r="D18" s="101" t="s">
         <v>380</v>
       </c>
-      <c r="E18" s="202" t="s">
+      <c r="E18" s="201" t="s">
         <v>382</v>
       </c>
       <c r="F18" s="38" t="s">
@@ -12152,7 +12168,7 @@
       <c r="I18" s="55"/>
     </row>
     <row r="19" spans="1:9" ht="22.5">
-      <c r="A19" s="189"/>
+      <c r="A19" s="188"/>
       <c r="B19" s="34" t="s">
         <v>38</v>
       </c>
@@ -12162,7 +12178,7 @@
       <c r="D19" s="103" t="s">
         <v>380</v>
       </c>
-      <c r="E19" s="204"/>
+      <c r="E19" s="203"/>
       <c r="F19" s="30" t="s">
         <v>417</v>
       </c>
@@ -12173,7 +12189,7 @@
       <c r="I19" s="55"/>
     </row>
     <row r="20" spans="1:9" ht="22.5">
-      <c r="A20" s="189"/>
+      <c r="A20" s="188"/>
       <c r="B20" s="50" t="s">
         <v>39</v>
       </c>
@@ -12196,7 +12212,7 @@
       <c r="I20" s="55"/>
     </row>
     <row r="21" spans="1:9" ht="22.5">
-      <c r="A21" s="189"/>
+      <c r="A21" s="188"/>
       <c r="B21" s="50" t="s">
         <v>40</v>
       </c>
@@ -12219,7 +12235,7 @@
       <c r="I21" s="55"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="190"/>
+      <c r="A22" s="189"/>
       <c r="B22" s="50" t="s">
         <v>42</v>
       </c>
@@ -12254,10 +12270,10 @@
       <c r="D23" s="105" t="s">
         <v>383</v>
       </c>
-      <c r="E23" s="202" t="s">
+      <c r="E23" s="201" t="s">
         <v>391</v>
       </c>
-      <c r="F23" s="205" t="s">
+      <c r="F23" s="204" t="s">
         <v>392</v>
       </c>
       <c r="G23" s="120" t="s">
@@ -12279,8 +12295,8 @@
       <c r="D24" s="107" t="s">
         <v>383</v>
       </c>
-      <c r="E24" s="203"/>
-      <c r="F24" s="206"/>
+      <c r="E24" s="202"/>
+      <c r="F24" s="205"/>
       <c r="G24" s="120" t="s">
         <v>211</v>
       </c>
@@ -12298,8 +12314,8 @@
       <c r="D25" s="107" t="s">
         <v>383</v>
       </c>
-      <c r="E25" s="203"/>
-      <c r="F25" s="206"/>
+      <c r="E25" s="202"/>
+      <c r="F25" s="205"/>
       <c r="G25" s="120" t="s">
         <v>212</v>
       </c>
@@ -12317,8 +12333,8 @@
       <c r="D26" s="109" t="s">
         <v>383</v>
       </c>
-      <c r="E26" s="204"/>
-      <c r="F26" s="207"/>
+      <c r="E26" s="203"/>
+      <c r="F26" s="206"/>
       <c r="G26" s="120" t="s">
         <v>213</v>
       </c>
@@ -12414,7 +12430,7 @@
       <c r="I30" s="55"/>
     </row>
     <row r="31" spans="1:9" ht="45">
-      <c r="A31" s="191" t="s">
+      <c r="A31" s="190" t="s">
         <v>47</v>
       </c>
       <c r="B31" s="50" t="s">
@@ -12436,7 +12452,7 @@
       <c r="I31" s="55"/>
     </row>
     <row r="32" spans="1:9" ht="120">
-      <c r="A32" s="192"/>
+      <c r="A32" s="191"/>
       <c r="B32" s="49" t="s">
         <v>48</v>
       </c>
@@ -12618,7 +12634,7 @@
       <c r="I39" s="54"/>
     </row>
     <row r="40" spans="1:11" ht="31.15" customHeight="1">
-      <c r="A40" s="191" t="s">
+      <c r="A40" s="190" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="50" t="s">
@@ -12643,7 +12659,7 @@
       <c r="I40" s="54"/>
     </row>
     <row r="41" spans="1:11" ht="31.9" customHeight="1">
-      <c r="A41" s="193"/>
+      <c r="A41" s="192"/>
       <c r="B41" s="50" t="s">
         <v>56</v>
       </c>
@@ -12653,7 +12669,7 @@
       <c r="D41" s="99" t="s">
         <v>380</v>
       </c>
-      <c r="E41" s="188" t="s">
+      <c r="E41" s="187" t="s">
         <v>396</v>
       </c>
       <c r="F41" s="38" t="s">
@@ -12666,7 +12682,7 @@
       <c r="I41" s="54"/>
     </row>
     <row r="42" spans="1:11" ht="23.45" customHeight="1">
-      <c r="A42" s="193"/>
+      <c r="A42" s="192"/>
       <c r="B42" s="50" t="s">
         <v>57</v>
       </c>
@@ -12676,7 +12692,7 @@
       <c r="D42" s="99" t="s">
         <v>380</v>
       </c>
-      <c r="E42" s="188"/>
+      <c r="E42" s="187"/>
       <c r="F42" s="38" t="s">
         <v>311</v>
       </c>
@@ -12687,7 +12703,7 @@
       <c r="I42" s="54"/>
     </row>
     <row r="43" spans="1:11" ht="34.9" customHeight="1">
-      <c r="A43" s="193"/>
+      <c r="A43" s="192"/>
       <c r="B43" s="50" t="s">
         <v>267</v>
       </c>
@@ -12697,7 +12713,7 @@
       <c r="D43" s="99" t="s">
         <v>380</v>
       </c>
-      <c r="E43" s="188"/>
+      <c r="E43" s="187"/>
       <c r="F43" s="38" t="s">
         <v>397</v>
       </c>
@@ -12708,7 +12724,7 @@
       <c r="K43" s="77"/>
     </row>
     <row r="44" spans="1:11" ht="22.5">
-      <c r="A44" s="193"/>
+      <c r="A44" s="192"/>
       <c r="B44" s="50" t="s">
         <v>58</v>
       </c>
@@ -12726,7 +12742,7 @@
       <c r="I44" s="54"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="193"/>
+      <c r="A45" s="192"/>
       <c r="B45" s="50" t="s">
         <v>59</v>
       </c>
@@ -12744,7 +12760,7 @@
       <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:11" ht="22.5">
-      <c r="A46" s="193"/>
+      <c r="A46" s="192"/>
       <c r="B46" s="50" t="s">
         <v>60</v>
       </c>
@@ -12762,7 +12778,7 @@
       <c r="I46" s="54"/>
     </row>
     <row r="47" spans="1:11" ht="22.5">
-      <c r="A47" s="193"/>
+      <c r="A47" s="192"/>
       <c r="B47" s="50" t="s">
         <v>61</v>
       </c>
@@ -12780,7 +12796,7 @@
       <c r="I47" s="54"/>
     </row>
     <row r="48" spans="1:11" ht="44.45" customHeight="1">
-      <c r="A48" s="193"/>
+      <c r="A48" s="192"/>
       <c r="B48" s="50" t="s">
         <v>62</v>
       </c>
@@ -12790,7 +12806,7 @@
       <c r="D48" s="99" t="s">
         <v>380</v>
       </c>
-      <c r="E48" s="188" t="s">
+      <c r="E48" s="187" t="s">
         <v>396</v>
       </c>
       <c r="F48" s="54"/>
@@ -12801,7 +12817,7 @@
       <c r="I48" s="54"/>
     </row>
     <row r="49" spans="1:9" ht="45.6" customHeight="1">
-      <c r="A49" s="192"/>
+      <c r="A49" s="191"/>
       <c r="B49" s="50" t="s">
         <v>63</v>
       </c>
@@ -12811,7 +12827,7 @@
       <c r="D49" s="99" t="s">
         <v>380</v>
       </c>
-      <c r="E49" s="188"/>
+      <c r="E49" s="187"/>
       <c r="F49" s="54"/>
       <c r="G49" s="120" t="s">
         <v>243</v>
@@ -12939,7 +12955,7 @@
       <c r="D55" s="99" t="s">
         <v>380</v>
       </c>
-      <c r="E55" s="188" t="s">
+      <c r="E55" s="187" t="s">
         <v>400</v>
       </c>
       <c r="F55" s="38" t="s">
@@ -12960,7 +12976,7 @@
       <c r="D56" s="99" t="s">
         <v>380</v>
       </c>
-      <c r="E56" s="188"/>
+      <c r="E56" s="187"/>
       <c r="F56" s="38" t="s">
         <v>315</v>
       </c>
@@ -12979,7 +12995,7 @@
       <c r="D57" s="111" t="s">
         <v>380</v>
       </c>
-      <c r="E57" s="188"/>
+      <c r="E57" s="187"/>
       <c r="F57" s="38" t="s">
         <v>401</v>
       </c>
@@ -13267,11 +13283,11 @@
       <c r="C5" s="54"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A6" s="208" t="s">
+      <c r="A6" s="207" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="208"/>
-      <c r="C6" s="208"/>
+      <c r="B6" s="207"/>
+      <c r="C6" s="207"/>
     </row>
     <row r="7" spans="1:3" ht="20.25" thickTop="1">
       <c r="A7" s="26" t="s">

</xml_diff>